<commit_message>
Added BRRequest middleware, Generic vies, mixins
</commit_message>
<xml_diff>
--- a/book/management/commands/uploads/book_list.xlsx
+++ b/book/management/commands/uploads/book_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="37">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -110,6 +110,27 @@
   </si>
   <si>
     <t xml:space="preserve">Jonathon Hack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Computer Science1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Computer Science2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Computer Science3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Computer Science4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Computer Science5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Computer Science6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Computer Science7</t>
   </si>
 </sst>
 </file>
@@ -120,7 +141,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M\-D\-YYYY"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -169,11 +190,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -224,7 +240,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -253,11 +269,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,23 +353,23 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="20" min="14" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="213.15306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="213.15306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="20" min="14" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="210.857142857143"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="210.857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,7 +513,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
@@ -548,7 +560,7 @@
       <c r="Q3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="S3" s="6" t="s">
@@ -569,7 +581,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>21</v>
@@ -616,7 +628,7 @@
       <c r="Q4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S4" s="6" t="s">
@@ -637,7 +649,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -684,7 +696,7 @@
       <c r="Q5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="R5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="S5" s="6" t="s">
@@ -705,7 +717,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>21</v>
@@ -752,7 +764,7 @@
       <c r="Q6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S6" s="6" t="s">
@@ -773,7 +785,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>21</v>
@@ -820,7 +832,7 @@
       <c r="Q7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="8" t="s">
+      <c r="R7" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S7" s="6" t="s">
@@ -841,7 +853,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
@@ -888,7 +900,7 @@
       <c r="Q8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R8" s="8" t="s">
+      <c r="R8" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S8" s="6" t="s">
@@ -909,7 +921,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
@@ -956,7 +968,7 @@
       <c r="Q9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R9" s="8" t="s">
+      <c r="R9" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S9" s="6" t="s">

</xml_diff>